<commit_message>
Colas Sin Azucar change has been made.
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Data/CCNayarTemplatev0.8.9.xlsx
+++ b/Projects/CCNAYARMX/Data/CCNayarTemplatev0.8.9.xlsx
@@ -63,6 +63,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$79</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatavase_1" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$J$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$J$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2219,7 +2220,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
+      <selection pane="bottomLeft" activeCell="F47" activeCellId="1" sqref="H4 F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2227,12 +2228,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.914979757085"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="130.46963562753"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="131.647773279352"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="11" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
@@ -4290,17 +4291,17 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="H4 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8866396761134"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4464,24 +4465,24 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="61" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="61" width="61.914979757085"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="55.4858299595142"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="61" width="65.9838056680162"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="94.9068825910931"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="61" width="65.9838056680162"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="61" width="98.5506072874494"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="61" width="71.7692307692308"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="61" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="55.914979757085"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="61" width="66.5222672064777"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="95.7651821862348"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="61" width="66.5222672064777"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="61" width="99.4048582995952"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="61" width="72.4129554655871"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="61" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="61" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="61" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="61" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="61" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="61" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="61" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="61" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="61" width="11.6761133603239"/>
@@ -4641,7 +4642,7 @@
       </c>
       <c r="S3" s="92"/>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>35</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>298</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>300</v>
+        <v>215</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="3" t="s">
@@ -4711,7 +4712,7 @@
         <v>298</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>300</v>
+        <v>215</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>197</v>
@@ -4803,21 +4804,21 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="H4 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.919028340081"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="96.5141700404858"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.1255060728745"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="97.3724696356275"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.7692307692308"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6761133603239"/>
@@ -5228,7 +5229,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="H4 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5352,19 +5353,19 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="H4 H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.8097165991903"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.1336032388664"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.0607287449393"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="49.3805668016194"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="56.7732793522267"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.3846153846154"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="49.7044534412956"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="57.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
@@ -5481,7 +5482,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="H4 G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5558,20 +5559,20 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="H4 B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="68.5546558704453"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="69.0931174089069"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10526315789474"/>
@@ -5755,27 +5756,27 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="H4 H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="84.5182186234818"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="85.2672064777328"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.9838056680162"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="54.7368421052632"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.0526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.5222672064777"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.6720647773279"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.8866396761134"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -6243,7 +6244,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="H4 E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6254,14 +6255,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.0971659919028"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.4210526315789"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
@@ -6385,17 +6386,17 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="1" sqref="H4 C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.3036437246964"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0526315789474"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="113.437246963563"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.8785425101215"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="114.404858299595"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -6650,20 +6651,20 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="H4 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="61" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="56.8785425101215"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="61" width="77.3400809716599"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="62.8785425101215"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="61" width="77.9838056680162"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="82.4817813765182"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="61" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="61" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="61" width="104.655870445344"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="61" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="61" width="105.619433198381"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="61" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="61" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="61" width="13.3886639676113"/>
@@ -7190,26 +7191,26 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+      <selection pane="topLeft" activeCell="N4" activeCellId="1" sqref="H4 N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="61.914979757085"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8461538461538"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="65.9838056680162"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="94.9068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="70.5910931174089"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="66.5222672064777"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="95.7651821862348"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="71.1255060728745"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="35.8866396761134"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
@@ -7418,24 +7419,24 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="H4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.0607287449393"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="68.9838056680162"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.6275303643725"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10526315789474"/>
   </cols>
@@ -7626,16 +7627,16 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="H4 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.6275303643725"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.2712550607288"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>